<commit_message>
Curves and tidy up
Adds updated curves to repo, and tidies up repo
</commit_message>
<xml_diff>
--- a/Input Data.xlsx
+++ b/Input Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reece\Documents\COMP3217CW2-20202021\CPS-Smart-Energy-Scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3135E7BE-925B-4114-884C-D5A30782CACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC14E5A-3360-4F56-A41B-5C73F676671A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21630" yWindow="7950" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="3" xr2:uid="{DE4D9E89-ED3E-9F4F-B454-34A6DA40E3CF}"/>
+    <workbookView xWindow="0" yWindow="5565" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="3" xr2:uid="{DE4D9E89-ED3E-9F4F-B454-34A6DA40E3CF}"/>
   </bookViews>
   <sheets>
     <sheet name="User &amp; Task ID" sheetId="1" r:id="rId1"/>
@@ -302,6 +302,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -357,7 +360,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -365,6 +368,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3003,9 +3009,6 @@
           <cell r="B18">
             <v>5.883769</v>
           </cell>
-          <cell r="E18" t="str">
-            <v xml:space="preserve">PAR </v>
-          </cell>
         </row>
         <row r="19">
           <cell r="A19">
@@ -3013,9 +3016,6 @@
           </cell>
           <cell r="B19">
             <v>6.3292630000000001</v>
-          </cell>
-          <cell r="E19">
-            <v>1.3291280000000001</v>
           </cell>
         </row>
         <row r="20">
@@ -4713,7 +4713,7 @@
   <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="B3:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4734,7 +4734,7 @@
       <c r="B3" t="s">
         <v>60</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.789333333333333</v>
       </c>
     </row>
@@ -4742,7 +4742,7 @@
       <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.94099999999999995</v>
       </c>
     </row>
@@ -4750,7 +4750,7 @@
       <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.94</v>
       </c>
     </row>
@@ -4758,7 +4758,7 @@
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>0.97733333333333305</v>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
       <c r="B7" t="s">
         <v>64</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>0.77133333333333298</v>
       </c>
     </row>
@@ -4774,7 +4774,7 @@
       <c r="B8" t="s">
         <v>65</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>0.73733333333333295</v>
       </c>
     </row>
@@ -4782,7 +4782,7 @@
       <c r="B9" t="s">
         <v>66</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>0.78900000000000003</v>
       </c>
     </row>
@@ -4790,7 +4790,7 @@
       <c r="B10" t="s">
         <v>67</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>0.92400000000000004</v>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
       <c r="B11" t="s">
         <v>68</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>0.94799999999999995</v>
       </c>
     </row>
@@ -4806,7 +4806,7 @@
       <c r="B12" t="s">
         <v>69</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>0.94899999999999995</v>
       </c>
     </row>

</xml_diff>